<commit_message>
added listing and grouping docs
</commit_message>
<xml_diff>
--- a/PPP-Lista_dokumentów.xlsx
+++ b/PPP-Lista_dokumentów.xlsx
@@ -17,13 +17,25 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="238"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +58,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normalny" xfId="0"/>
@@ -360,36 +385,226 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A11:A11"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="M13" pane="bottomLeft" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" style="2" width="50.7109375"/>
+    <col customWidth="1" max="2" min="2" style="4" width="9.140625"/>
+    <col customWidth="1" max="16384" min="3" style="3" width="9.140625"/>
+  </cols>
   <sheetData>
-    <row hidden="1" outlineLevel="1" r="4"/>
-    <row hidden="1" outlineLevel="1" r="5"/>
-    <row hidden="1" outlineLevel="1" r="6"/>
-    <row hidden="1" outlineLevel="1" r="7"/>
-    <row hidden="1" outlineLevel="1" r="8"/>
-    <row hidden="1" outlineLevel="1" r="9"/>
-    <row hidden="1" outlineLevel="1" r="10"/>
-    <row hidden="1" outlineLevel="2" r="11">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nr_dokumentu.rewizja-Nazwa_dokumentu</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Nr KZ</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="1" r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>01-00-Rejestr_numerów_elementów.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="1" r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1.01.00-Podstawa.ipt</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="1" r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1.02.01-Wspornik_czujników_odległości.ipt</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="1" r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1.03.00-Wspornik_ogniwa.ipt</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="1" r="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>2.00-Inteligentny_pojazd</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="2" r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Metals.Ornamental Metals.Chrome.Satin.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="1" r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2.00.01-Inteligentny_pojazd.iam</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="1" r="9">
+      <c r="A9" s="5" t="inlineStr">
+        <is>
+          <t>Archiwum</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="2" r="10">
+      <c r="A10" s="5" t="inlineStr">
+        <is>
+          <t>2019-01-07</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="3" r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Twoja stara</t>
-        </is>
-      </c>
-    </row>
-    <row hidden="1" outlineLevel="2" r="12"/>
-    <row hidden="1" outlineLevel="2" r="13"/>
-    <row hidden="1" outlineLevel="2" r="14"/>
-    <row hidden="1" outlineLevel="1" r="15"/>
+          <t>2.00-Inteligentny_pojazd.iam</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="2" r="12">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>2019-03-10</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="3" r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1.01-Podstawa.ipt</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="3" r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1.02-Wspornik_czujników_odległości.ipt</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="3" r="15">
+      <c r="A15" s="5" t="inlineStr">
+        <is>
+          <t>3_poziom</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="4" r="16">
+      <c r="A16" s="5" t="inlineStr">
+        <is>
+          <t>4_poziom</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="5" r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Nowy Archiwum WinRARa.rar</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="5" r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Nowy obraz mapy bitowej.bmp</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="4" r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Nowy Dokument programu Microsoft Word.docx</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="4" r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Nowy dokument tekstowy.txt</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="4" r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Nowy obraz mapy bitowej.bmp</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="1" r="22">
+      <c r="A22" s="5" t="inlineStr">
+        <is>
+          <t>OldVersions</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="2" r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>1.01-Podstawa.0012.ipt</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="2" r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>1.01.00-Podstawa.0016.ipt</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="2" r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>1.02-Wspornik_czujników_odległości.0020.ipt</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="2" r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2.00-Inteligentny_pojazd.0003.iam</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="2" r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2.00-Inteligentny_pojazd.0019.iam</t>
+        </is>
+      </c>
+    </row>
+    <row hidden="1" outlineLevel="2" r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2.00.01-Inteligentny_pojazd.0013.iam</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added kz number filling
</commit_message>
<xml_diff>
--- a/PPP-Lista_dokumentów.xlsx
+++ b/PPP-Lista_dokumentów.xlsx
@@ -392,13 +392,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="M13" pane="bottomLeft" sqref="M13"/>
+      <selection activeCell="F11" pane="bottomLeft" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="2" width="50.7109375"/>
-    <col customWidth="1" max="2" min="2" style="4" width="9.140625"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="4" width="10"/>
     <col customWidth="1" max="16384" min="3" style="3" width="9.140625"/>
   </cols>
   <sheetData>
@@ -420,6 +420,11 @@
           <t>01-00-Rejestr_numerów_elementów.xlsx</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="1" r="3">
       <c r="A3" t="inlineStr">
@@ -427,6 +432,11 @@
           <t>1.01.00-Podstawa.ipt</t>
         </is>
       </c>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>5123, PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="1" r="4">
       <c r="A4" t="inlineStr">
@@ -434,6 +444,11 @@
           <t>1.02.01-Wspornik_czujników_odległości.ipt</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="1" r="5">
       <c r="A5" t="inlineStr">
@@ -441,6 +456,11 @@
           <t>1.03.00-Wspornik_ogniwa.ipt</t>
         </is>
       </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>321, PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="1" r="6">
       <c r="A6" s="5" t="inlineStr">
@@ -455,6 +475,11 @@
           <t>Metals.Ornamental Metals.Chrome.Satin.jpg</t>
         </is>
       </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>423, PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="1" r="8">
       <c r="A8" t="inlineStr">
@@ -462,6 +487,11 @@
           <t>2.00.01-Inteligentny_pojazd.iam</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="1" r="9">
       <c r="A9" s="5" t="inlineStr">
@@ -483,6 +513,11 @@
           <t>2.00-Inteligentny_pojazd.iam</t>
         </is>
       </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>1523, PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="2" r="12">
       <c r="A12" s="5" t="inlineStr">
@@ -497,6 +532,11 @@
           <t>1.01-Podstawa.ipt</t>
         </is>
       </c>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>1234, PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="3" r="14">
       <c r="A14" t="inlineStr">
@@ -504,6 +544,11 @@
           <t>1.02-Wspornik_czujników_odległości.ipt</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="3" r="15">
       <c r="A15" s="5" t="inlineStr">
@@ -525,6 +570,11 @@
           <t>Nowy Archiwum WinRARa.rar</t>
         </is>
       </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="5" r="18">
       <c r="A18" t="inlineStr">
@@ -532,6 +582,11 @@
           <t>Nowy obraz mapy bitowej.bmp</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="4" r="19">
       <c r="A19" t="inlineStr">
@@ -539,6 +594,11 @@
           <t>Nowy Dokument programu Microsoft Word.docx</t>
         </is>
       </c>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t>1235, PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="4" r="20">
       <c r="A20" t="inlineStr">
@@ -546,6 +606,11 @@
           <t>Nowy dokument tekstowy.txt</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="4" r="21">
       <c r="A21" t="inlineStr">
@@ -553,6 +618,11 @@
           <t>Nowy obraz mapy bitowej.bmp</t>
         </is>
       </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="1" r="22">
       <c r="A22" s="5" t="inlineStr">
@@ -567,6 +637,11 @@
           <t>1.01-Podstawa.0012.ipt</t>
         </is>
       </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="2" r="24">
       <c r="A24" t="inlineStr">
@@ -574,6 +649,11 @@
           <t>1.01.00-Podstawa.0016.ipt</t>
         </is>
       </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="2" r="25">
       <c r="A25" t="inlineStr">
@@ -581,6 +661,11 @@
           <t>1.02-Wspornik_czujników_odległości.0020.ipt</t>
         </is>
       </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="2" r="26">
       <c r="A26" t="inlineStr">
@@ -588,6 +673,11 @@
           <t>2.00-Inteligentny_pojazd.0003.iam</t>
         </is>
       </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="2" r="27">
       <c r="A27" t="inlineStr">
@@ -595,11 +685,21 @@
           <t>2.00-Inteligentny_pojazd.0019.iam</t>
         </is>
       </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>PPP-NNN</t>
+        </is>
+      </c>
     </row>
     <row hidden="1" outlineLevel="2" r="28">
       <c r="A28" t="inlineStr">
         <is>
           <t>2.00.01-Inteligentny_pojazd.0013.iam</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>PPP-NNN</t>
         </is>
       </c>
     </row>

</xml_diff>